<commit_message>
start to convert to package
</commit_message>
<xml_diff>
--- a/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,25 +3,26 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="10" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="16" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="18" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="23" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="24" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="5" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="6" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="9" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="15" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="151" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="152" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="18" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -48,7 +49,7 @@
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2346,7 +2347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2376,11 +2377,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -2438,17 +2439,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.5245319561007101</v>
+        <v>0.7914893617021277</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.4118416589951063</v>
+        <v>0.912538516236075</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -2458,11 +2459,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>زانوسي العبد 309 - 314</t>
+          <t>LG43LM63-UM73</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -2582,17 +2583,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="30" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>صندوق سمك 25 ك</t>
+          <t>فوم زوايا فيكتوريا اماميه وخلفية</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -2602,11 +2603,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>فوم  60*90 (دعامة و قاعدة)</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -2717,10 +2718,10 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="29" t="n">
-        <v>6</v>
-      </c>
-      <c r="B25" s="30" t="n"/>
+      <c r="A25" s="29" t="n"/>
+      <c r="B25" s="30" t="n">
+        <v>1</v>
+      </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
@@ -2831,17 +2832,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>قاعدة غسالة Lg</t>
+          <t>قاعدة وزوايا كولدير ميلو</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -2850,28 +2851,16 @@
     <row r="36" ht="18" customHeight="1">
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D36" s="18" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="18" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="D37" s="18" t="inlineStr">
-        <is>
-          <t>فوم كوش 152</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -2914,6 +2903,611 @@
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F42" sqref="A1:F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="26.625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.25" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.625" customWidth="1" min="3" max="3"/>
+    <col width="20.125" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.875" customWidth="1" min="5" max="5"/>
+    <col width="31.875" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="31" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="32" t="n"/>
+      <c r="C2" s="36" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="37" t="n"/>
+      <c r="E2" s="37" t="n"/>
+      <c r="F2" s="37" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="34" t="n">
+        <v>0.6740049453617293</v>
+      </c>
+      <c r="B4" s="35" t="n">
+        <v>0.6012506012506013</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG75UP77set</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+    </row>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG Nano80</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="18" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="4" t="n"/>
+      <c r="D8" s="18" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="18" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="18" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="19" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D12" s="39" t="n"/>
+      <c r="E12" s="39" t="n"/>
+      <c r="F12" s="39" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D13" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="29" t="n">
+        <v>9</v>
+      </c>
+      <c r="B14" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="27" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>جانب حماية يمين / شمال</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="27" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="27" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="27" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="27" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="18" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="27" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="27" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="18" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="20" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="33" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="39" t="n"/>
+      <c r="E23" s="39" t="n"/>
+      <c r="F23" s="39" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="29" t="n">
+        <v>10</v>
+      </c>
+      <c r="B25" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="27" t="n"/>
+      <c r="C26" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="27" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="18" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="27" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="18" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="27" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="18" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="27" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="18" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="27" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="18" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="27" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="19" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="33" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="39" t="n"/>
+      <c r="E33" s="39" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="B35" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="n"/>
+      <c r="D35" s="18" t="n"/>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="27" t="n"/>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="18" t="n"/>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="27" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="27" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="27" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="18" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="27" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="18" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="27" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="18" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="28" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="19" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2947,8 +3541,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -2969,11 +3563,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -3031,17 +3625,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.712523979172376</v>
+        <v>0.9302671727320087</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.828438017773761</v>
+        <v>0.6442617433530459</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>صندوق 10 ك فلات</t>
+          <t>LG75UP77set</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -3051,11 +3645,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>زانوسى العبد 305-جديدة</t>
+          <t>LG Nano80</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -3072,14 +3666,8 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" s="18" t="inlineStr">
-        <is>
-          <t>LG65UP77_TB</t>
-        </is>
-      </c>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="18" t="n"/>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
@@ -3181,17 +3769,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B14" s="30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>بوتجاز  90 تصدير</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -3201,11 +3789,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -3214,14 +3802,8 @@
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D16" s="18" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
-        </is>
-      </c>
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="18" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
@@ -3323,17 +3905,11 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="29" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B25" s="30" t="n"/>
-      <c r="C25" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D25" s="18" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -3442,17 +4018,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -3462,11 +4038,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -3475,14 +4051,8 @@
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="D37" s="18" t="inlineStr">
-        <is>
-          <t>فوم كوش 152</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -3580,11 +4150,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -3642,17 +4212,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.7400714254980423</v>
+        <v>0.7685762125662211</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.9533839587606008</v>
+        <v>0.7185001903311762</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+          <t>LG75UP77set</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -3662,11 +4232,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>LG Nano80</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -3683,16 +4253,28 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة غسالة Lg</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
@@ -3786,17 +4368,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>6</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -3806,11 +4388,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -3819,16 +4401,28 @@
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 5ك بنى سويف</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
@@ -3922,7 +4516,7 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="29" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n">
@@ -3930,7 +4524,7 @@
       </c>
       <c r="D25" s="18" t="inlineStr">
         <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
+          <t>زوايا غسالة كليوباترا</t>
         </is>
       </c>
       <c r="E25" s="9" t="n"/>
@@ -4047,17 +4641,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -4066,28 +4660,16 @@
     <row r="36" ht="18" customHeight="1">
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D36" s="18" t="inlineStr">
-        <is>
-          <t>LG 65UP77 FRONT</t>
-        </is>
-      </c>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="18" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D37" s="18" t="inlineStr">
-        <is>
-          <t>LG65UM73</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -4185,11 +4767,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -4247,17 +4829,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.5386377131224023</v>
+        <v>10.55251938539014</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.6558220279045843</v>
+        <v>10.81323109643477</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -4267,11 +4849,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>OLED65cs6la</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -4289,11 +4871,11 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="18" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E6" s="9" t="n"/>
@@ -4302,16 +4884,28 @@
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>صندوق 10 ك فلات</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>جوانب بوتجاز يمين وشمال</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -4326,16 +4920,28 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="18" t="n"/>
+      <c r="C9" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
     <row r="10" ht="18" customHeight="1">
       <c r="A10" s="13" t="n"/>
       <c r="B10" s="15" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="18" t="n"/>
+      <c r="C10" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D10" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
@@ -4397,17 +5003,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="30" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="n">
-        <v>6</v>
-      </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>LG 65UP77 FRONT</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -4417,11 +5023,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+          <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -4430,32 +5036,56 @@
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 10بنى سويف</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="27" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="18" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
       <c r="A19" s="24" t="n"/>
       <c r="B19" s="27" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="18" t="n"/>
+      <c r="C19" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D19" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
@@ -4533,15 +5163,15 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="29" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" s="18" t="inlineStr">
         <is>
-          <t>صندوق سمك 5ك بنى سويف</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E25" s="9" t="n"/>
@@ -4550,14 +5180,8 @@
     <row r="26" ht="18" customHeight="1">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="27" t="n"/>
-      <c r="C26" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D26" s="18" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 3 اطقم</t>
-        </is>
-      </c>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="18" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
@@ -4658,17 +5282,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>OLED65cs6la</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -4678,11 +5302,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -4691,28 +5315,16 @@
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D37" s="18" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
       <c r="A38" s="24" t="n"/>
       <c r="B38" s="27" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="D38" s="18" t="inlineStr">
-        <is>
-          <t>فوم كوش 130</t>
-        </is>
-      </c>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
@@ -4780,8 +5392,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -4802,11 +5414,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -4864,17 +5476,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.7547330718062425</v>
+        <v>1.345344400298965</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.7648183556405354</v>
+        <v>2.020844935953536</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>LG43UP79</t>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -4884,11 +5496,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>LG75UP77-front</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -4905,24 +5517,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>OLED65cs6la</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP81</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -4937,24 +5567,42 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="18" t="n"/>
+      <c r="C9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>فوم  60*90 (دعامة و قاعدة)</t>
+        </is>
+      </c>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
     <row r="10" ht="18" customHeight="1">
       <c r="A10" s="13" t="n"/>
       <c r="B10" s="15" t="n"/>
-      <c r="C10" s="4" t="n"/>
-      <c r="D10" s="18" t="n"/>
+      <c r="C10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
     </row>
     <row r="11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A11" s="13" t="n"/>
       <c r="B11" s="15" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="19" t="n"/>
+      <c r="C11" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="D11" s="19" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
     </row>
@@ -5008,17 +5656,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" s="30" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>LG43UP79</t>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -5028,11 +5676,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -5042,11 +5690,11 @@
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D16" s="18" t="inlineStr">
         <is>
-          <t>oled55cs6la</t>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -5055,32 +5703,56 @@
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 10بنى سويف</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="27" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="18" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>فوم  60*90 (دعامة و قاعدة)</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
       <c r="A19" s="24" t="n"/>
       <c r="B19" s="27" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="18" t="n"/>
+      <c r="C19" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D19" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
       <c r="A20" s="24" t="n"/>
       <c r="B20" s="27" t="n"/>
-      <c r="C20" s="4" t="n"/>
-      <c r="D20" s="18" t="n"/>
+      <c r="C20" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D20" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 4 اطقم</t>
+        </is>
+      </c>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
@@ -5150,11 +5822,19 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="29" t="n">
-        <v>4</v>
-      </c>
-      <c r="B25" s="30" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="18" t="n"/>
+        <v>9</v>
+      </c>
+      <c r="B25" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>طقم سخان نبتون ذو 3 اطقم</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -5263,17 +5943,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LG43UP79</t>
+          <t>LG 65UP77 FRONT</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -5283,11 +5963,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>LG65UP81</t>
+          <t>OLED65cs6la</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -5297,11 +5977,11 @@
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>قاعدة غسالة Lg</t>
+          <t>صندوق سمك 10بنى سويف</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
@@ -5311,11 +5991,11 @@
       <c r="A38" s="24" t="n"/>
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="4" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D38" s="18" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>LG65UM73</t>
         </is>
       </c>
       <c r="E38" s="9" t="n"/>
@@ -5324,56 +6004,32 @@
     <row r="39" ht="18" customHeight="1">
       <c r="A39" s="24" t="n"/>
       <c r="B39" s="27" t="n"/>
-      <c r="C39" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D39" s="18" t="inlineStr">
-        <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
-        </is>
-      </c>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
       <c r="A40" s="24" t="n"/>
       <c r="B40" s="27" t="n"/>
-      <c r="C40" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D40" s="18" t="inlineStr">
-        <is>
-          <t>oled55cs6la</t>
-        </is>
-      </c>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
       <c r="A41" s="24" t="n"/>
       <c r="B41" s="27" t="n"/>
-      <c r="C41" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="D41" s="18" t="inlineStr">
-        <is>
-          <t>فوم كشاف طوارئ جراند 1</t>
-        </is>
-      </c>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="18" t="n"/>
       <c r="E41" s="9" t="n"/>
       <c r="F41" s="9" t="n"/>
     </row>
     <row r="42" ht="18.75" customHeight="1" thickBot="1">
       <c r="A42" s="25" t="n"/>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="D42" s="19" t="inlineStr">
-        <is>
-          <t>فوم كوش 130</t>
-        </is>
-      </c>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
     </row>
@@ -5409,8 +6065,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -5431,11 +6087,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -5493,17 +6149,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>1.70760934691432</v>
+        <v>0.7913175559802048</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>1.55217965653897</v>
+        <v>0.9616550163642976</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>LG43UP79</t>
+          <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -5513,11 +6169,11 @@
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LG65UM73</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -5534,24 +6190,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -5566,8 +6240,14 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="18" t="n"/>
+      <c r="C9" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>سخان غاز 6لتر</t>
+        </is>
+      </c>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
@@ -5637,17 +6317,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="30" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>فكتوريا قاعدة ولوحة تحكم وحلة</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -5656,32 +6336,56 @@
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 23ك فلات</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="27" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="18" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
@@ -5767,7 +6471,7 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="29" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n"/>
@@ -5880,17 +6584,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B35" s="26" t="n">
         <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LG65UP81</t>
+          <t>صندوق سمك 23ك فلات</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -5900,11 +6604,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>كفر غسالة LG/زوايا غسالة LG</t>
+          <t>LG65UM73</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -5914,11 +6618,11 @@
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>LG65UM73</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
@@ -6018,11 +6722,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -6080,17 +6784,17 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.5092649404834949</v>
+        <v>0.7913175559802048</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.4497269514937359</v>
+        <v>0.9616550163642976</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>LG75UP77set</t>
+          <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
@@ -6104,7 +6808,7 @@
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -6121,24 +6825,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -6153,8 +6875,14 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="18" t="n"/>
+      <c r="C9" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>سخان غاز 6لتر</t>
+        </is>
+      </c>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
@@ -6227,14 +6955,14 @@
         <v>11</v>
       </c>
       <c r="B14" s="30" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>فكتوريا قاعدة ولوحة تحكم وحلة</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -6243,32 +6971,56 @@
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 23ك فلات</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="27" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="18" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
@@ -6353,10 +7105,10 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="29" t="n"/>
-      <c r="B25" s="30" t="n">
-        <v>1</v>
-      </c>
+      <c r="A25" s="29" t="n">
+        <v>13</v>
+      </c>
+      <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
@@ -6467,17 +7219,17 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>فوم كشاف جراند بلاستيك</t>
+          <t>صندوق سمك 23ك فلات</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -6486,16 +7238,28 @@
     <row r="36" ht="18" customHeight="1">
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="18" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="18" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
@@ -6593,11 +7357,11 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C1" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -6655,21 +7419,33 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.3582297742835405</v>
+        <v>0.7913175559802048</v>
       </c>
       <c r="B4" s="35" t="n">
-        <v>0.4020451863829043</v>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+        <v>0.9616550163642976</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="27" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -6684,24 +7460,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LgWashing Mashine Base (VIVACHE)</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -6716,8 +7510,14 @@
           <t>وسيط التوالف</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="18" t="n"/>
+      <c r="C9" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="18" t="inlineStr">
+        <is>
+          <t>سخان غاز 6لتر</t>
+        </is>
+      </c>
       <c r="E9" s="9" t="n"/>
       <c r="F9" s="9" t="n"/>
     </row>
@@ -6787,17 +7587,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="29" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="30" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>فكتوريا قاعدة ولوحة تحكم وحلة</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -6807,11 +7607,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="27" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>LG32LM55-LM63</t>
+          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -6820,24 +7620,42 @@
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="27" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 23ك فلات</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="27" t="n"/>
-      <c r="C17" s="4" t="n"/>
-      <c r="D17" s="18" t="n"/>
+      <c r="C17" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="27" t="n"/>
-      <c r="C18" s="4" t="n"/>
-      <c r="D18" s="18" t="n"/>
+      <c r="C18" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
@@ -6922,10 +7740,10 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="29" t="n"/>
-      <c r="B25" s="30" t="n">
-        <v>1</v>
-      </c>
+      <c r="A25" s="29" t="n">
+        <v>13</v>
+      </c>
+      <c r="B25" s="30" t="n"/>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
@@ -7039,14 +7857,14 @@
         <v>13</v>
       </c>
       <c r="B35" s="26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>LgWashing Mashine Base (VIVACHE)</t>
+          <t>صندوق سمك 23ك فلات</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -7055,16 +7873,28 @@
     <row r="36" ht="18" customHeight="1">
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="27" t="n"/>
-      <c r="C36" s="4" t="n"/>
-      <c r="D36" s="18" t="n"/>
+      <c r="C36" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>LG65UM73</t>
+        </is>
+      </c>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="27" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="18" t="n"/>
+      <c r="C37" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>

</xml_diff>

<commit_message>
close some file to can integrate to another project
</commit_message>
<xml_diff>
--- a/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/analysis/formats/QC_molds_daily_summary.xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
-    <sheet name="5" sheetId="2" r:id="rId2"/>
-    <sheet name="6" sheetId="3" r:id="rId3"/>
-    <sheet name="11" sheetId="4" r:id="rId4"/>
-    <sheet name="12" sheetId="5" r:id="rId5"/>
-    <sheet name="13" sheetId="7" r:id="rId6"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
+    <sheet name="5" sheetId="4" r:id="rId4"/>
+    <sheet name="10" sheetId="5" r:id="rId5"/>
+    <sheet name="11" sheetId="6" r:id="rId6"/>
+    <sheet name="12" sheetId="7" r:id="rId7"/>
+    <sheet name="17" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">daily!$A$2:$F$2</definedName>
@@ -51,12 +53,12 @@
     <definedName name="Year">'[4]Incom Statment'!#REF!</definedName>
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="59">
   <si>
     <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
   </si>
@@ -121,85 +123,118 @@
     <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
   </si>
   <si>
-    <t>5</t>
+    <t>LG65UP77_TB</t>
   </si>
   <si>
-    <t>LG Nano80</t>
+    <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
+  </si>
+  <si>
+    <t>LG65UP81</t>
+  </si>
+  <si>
+    <t>LG43LM63-UM73</t>
+  </si>
+  <si>
+    <t>طقم اوجينى نجواى 69</t>
+  </si>
+  <si>
+    <t>فوم كوش 130</t>
+  </si>
+  <si>
+    <t>طقم سخان نبتون ذو 4 اطقم</t>
+  </si>
+  <si>
+    <t>فوم  60*90 (دعامة و قاعدة)</t>
+  </si>
+  <si>
+    <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+  </si>
+  <si>
+    <t>طقم سخان نبتون ذو 3 اطقم</t>
+  </si>
+  <si>
+    <t>(إفتا)S1B1</t>
+  </si>
+  <si>
+    <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+  </si>
+  <si>
+    <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+  </si>
+  <si>
+    <t>قاعدة غسالة Lg</t>
+  </si>
+  <si>
+    <t>فوم طقم رويال جاز المعدل</t>
+  </si>
+  <si>
+    <t>زوايا غسالة كليوباترا</t>
+  </si>
+  <si>
+    <t>جوانب بوتجاز يمين وشمال</t>
+  </si>
+  <si>
+    <t>75QNED81 UR91</t>
+  </si>
+  <si>
+    <t>OLED65A2</t>
+  </si>
+  <si>
+    <t>كفر غسالة LG/زوايا غسالة LG</t>
+  </si>
+  <si>
+    <t>LG65UM73</t>
+  </si>
+  <si>
+    <t>فوم صندوق سمك 35 ك</t>
+  </si>
+  <si>
+    <t>LG 65QNED81</t>
+  </si>
+  <si>
+    <t>LG43UP79</t>
+  </si>
+  <si>
+    <t>LG75UP77set</t>
+  </si>
+  <si>
+    <t>LG75UP77-front</t>
+  </si>
+  <si>
+    <t>صندوق سمك 25 ك</t>
+  </si>
+  <si>
+    <t>(إفتا)SAB</t>
+  </si>
+  <si>
+    <t>oled55cs6la</t>
+  </si>
+  <si>
+    <t>مبرد 70 لتر ك16</t>
+  </si>
+  <si>
+    <t>OLED65cs6la</t>
+  </si>
+  <si>
+    <t>فوم قاعده 60*60</t>
+  </si>
+  <si>
+    <t>قاعدة غسالة كيلوباترا</t>
+  </si>
+  <si>
+    <t>صندوق سمك 10بنى سويف</t>
+  </si>
+  <si>
+    <t>فوم حمايةالعداد2</t>
   </si>
   <si>
     <t>LgWashing Mashine Base (VIVACHE)</t>
   </si>
   <si>
-    <t>LG43LM63-UM73</t>
-  </si>
-  <si>
-    <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
-  </si>
-  <si>
-    <t>LG65UP77_TB</t>
-  </si>
-  <si>
-    <t>LG65UP81</t>
-  </si>
-  <si>
-    <t>فوم قاعده 60*60</t>
+    <t>صندوق سمك 23ك فلات</t>
   </si>
   <si>
     <t>Stop Coller S4</t>
-  </si>
-  <si>
-    <t>LG65UM73</t>
-  </si>
-  <si>
-    <t>كفر غسالة LG/زوايا غسالة LG</t>
-  </si>
-  <si>
-    <t>فوم حمايةالعداد2</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>OLED65A2</t>
-  </si>
-  <si>
-    <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-  </si>
-  <si>
-    <t>فوم دعامه 60*60</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>LG75UP77set</t>
-  </si>
-  <si>
-    <t>زوايا غسالة كليوباترا</t>
-  </si>
-  <si>
-    <t>فوم  60*90 (دعامة و قاعدة)</t>
-  </si>
-  <si>
-    <t>صندوق سمك 25 ك</t>
-  </si>
-  <si>
-    <t>غطاء صندوق سمك 20 ك فلات الجديدة</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>قاعدة غسالة Lg</t>
-  </si>
-  <si>
-    <t>جوانب بوتجاز يمين وشمال</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>FRONT 43LM63</t>
   </si>
 </sst>
 </file>
@@ -2334,7 +2369,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2353,11 +2388,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
+      <c r="B1" s="2">
+        <v>1</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="16">
         <v>2023</v>
@@ -2399,16 +2434,16 @@
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
-        <v>1.251665381109319</v>
+        <v>1.6756141207092889</v>
       </c>
       <c r="B4" s="30">
-        <v>1.0927938054202571</v>
+        <v>1.5982917044130971</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2417,10 +2452,10 @@
       <c r="A5" s="24"/>
       <c r="B5" s="31"/>
       <c r="C5" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2433,10 +2468,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2445,10 +2480,10 @@
       <c r="A7" s="13"/>
       <c r="B7" s="15"/>
       <c r="C7" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2457,10 +2492,10 @@
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -2473,10 +2508,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="4">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -2485,10 +2520,10 @@
       <c r="A10" s="13"/>
       <c r="B10" s="15"/>
       <c r="C10" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -2535,16 +2570,16 @@
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B14" s="36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -2553,7 +2588,7 @@
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="4">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>29</v>
@@ -2564,32 +2599,48 @@
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="4">
+        <v>6</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="4">
+        <v>25</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="4">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="31"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="4">
+        <v>49</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
@@ -2651,15 +2702,11 @@
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="36"/>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>22</v>
-      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
@@ -2752,16 +2799,16 @@
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -2770,10 +2817,10 @@
       <c r="A36" s="24"/>
       <c r="B36" s="31"/>
       <c r="C36" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -2782,10 +2829,10 @@
       <c r="A37" s="24"/>
       <c r="B37" s="31"/>
       <c r="C37" s="4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -2794,10 +2841,10 @@
       <c r="A38" s="24"/>
       <c r="B38" s="31"/>
       <c r="C38" s="4">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -2806,10 +2853,10 @@
       <c r="A39" s="24"/>
       <c r="B39" s="31"/>
       <c r="C39" s="4">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -2818,10 +2865,10 @@
       <c r="A40" s="24"/>
       <c r="B40" s="31"/>
       <c r="C40" s="4">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -2829,12 +2876,8 @@
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="31"/>
-      <c r="C41" s="4">
-        <v>25</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>32</v>
-      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
     </row>
@@ -2872,10 +2915,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A27" workbookViewId="0">
       <selection sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
@@ -2893,11 +2936,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>33</v>
+      <c r="B1" s="2">
+        <v>3</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="16">
         <v>2023</v>
@@ -2939,16 +2982,16 @@
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
-        <v>1.331360946745562</v>
+        <v>1.0972618179407281</v>
       </c>
       <c r="B4" s="30">
-        <v>0.95971713600202047</v>
+        <v>1.756500774926812</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2957,10 +3000,10 @@
       <c r="A5" s="24"/>
       <c r="B5" s="31"/>
       <c r="C5" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2973,10 +3016,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2985,10 +3028,10 @@
       <c r="A7" s="13"/>
       <c r="B7" s="15"/>
       <c r="C7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2997,10 +3040,10 @@
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -3013,10 +3056,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="4">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -3071,16 +3114,16 @@
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="36">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="4">
-        <v>49</v>
-      </c>
       <c r="D14" s="18" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -3088,32 +3131,48 @@
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="4">
+        <v>47</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="4">
+        <v>49</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
@@ -3183,14 +3242,14 @@
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -3284,16 +3343,16 @@
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35" s="32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -3302,10 +3361,10 @@
       <c r="A36" s="24"/>
       <c r="B36" s="31"/>
       <c r="C36" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -3314,10 +3373,10 @@
       <c r="A37" s="24"/>
       <c r="B37" s="31"/>
       <c r="C37" s="4">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -3326,10 +3385,10 @@
       <c r="A38" s="24"/>
       <c r="B38" s="31"/>
       <c r="C38" s="4">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -3337,12 +3396,8 @@
     <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="31"/>
-      <c r="C39" s="4">
-        <v>49</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>
@@ -3415,11 +3470,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>37</v>
+      <c r="B1" s="2">
+        <v>5</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="16">
         <v>2023</v>
@@ -3461,16 +3516,16 @@
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
-        <v>0.62219695534078712</v>
+        <v>0.78917700112739564</v>
       </c>
       <c r="B4" s="30">
-        <v>0.66537410769366356</v>
+        <v>0.96621055571069536</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -3478,12 +3533,8 @@
     <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="31"/>
-      <c r="C5" s="4">
-        <v>6</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>38</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
@@ -3577,16 +3628,16 @@
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" s="36">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
       <c r="D14" s="18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -3595,10 +3646,10 @@
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="4">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -3607,10 +3658,10 @@
       <c r="A16" s="24"/>
       <c r="B16" s="31"/>
       <c r="C16" s="4">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -3618,24 +3669,16 @@
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>41</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="4">
-        <v>49</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
@@ -3705,14 +3748,14 @@
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -3806,7 +3849,7 @@
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B35" s="32">
         <v>3</v>
@@ -3815,7 +3858,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -3827,7 +3870,7 @@
         <v>49</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -3909,7 +3952,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection sqref="A1:F42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3925,11 +3970,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
+      <c r="B1" s="2">
+        <v>10</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="16">
         <v>2023</v>
@@ -3971,16 +4016,16 @@
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
-        <v>0.95095629874986631</v>
+        <v>1.2794759825327511</v>
       </c>
       <c r="B4" s="30">
-        <v>0.91379040258994304</v>
+        <v>1.713786704508242</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -3989,10 +4034,10 @@
       <c r="A5" s="24"/>
       <c r="B5" s="31"/>
       <c r="C5" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -4005,10 +4050,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -4017,10 +4062,10 @@
       <c r="A7" s="13"/>
       <c r="B7" s="15"/>
       <c r="C7" s="4">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -4028,8 +4073,12 @@
     <row r="8" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="18"/>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
@@ -4040,24 +4089,36 @@
       <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="4">
+        <v>7</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="5">
+        <v>9</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
@@ -4095,16 +4156,16 @@
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B14" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -4113,10 +4174,10 @@
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -4128,7 +4189,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -4137,10 +4198,10 @@
       <c r="A17" s="24"/>
       <c r="B17" s="31"/>
       <c r="C17" s="4">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -4148,16 +4209,24 @@
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="4">
+        <v>47</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="31"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="4">
+        <v>49</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
@@ -4219,7 +4288,7 @@
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="4"/>
@@ -4316,16 +4385,16 @@
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B35" s="32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C35" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -4334,10 +4403,10 @@
       <c r="A36" s="24"/>
       <c r="B36" s="31"/>
       <c r="C36" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -4346,10 +4415,10 @@
       <c r="A37" s="24"/>
       <c r="B37" s="31"/>
       <c r="C37" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -4358,10 +4427,10 @@
       <c r="A38" s="24"/>
       <c r="B38" s="31"/>
       <c r="C38" s="4">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -4370,10 +4439,10 @@
       <c r="A39" s="24"/>
       <c r="B39" s="31"/>
       <c r="C39" s="4">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -4381,16 +4450,24 @@
     <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="31"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="18"/>
+      <c r="C40" s="4">
+        <v>48</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="31"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="18"/>
+      <c r="C41" s="4">
+        <v>49</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
     </row>
@@ -4431,7 +4508,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
@@ -4449,11 +4526,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>46</v>
+      <c r="B1" s="2">
+        <v>11</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="16">
         <v>2023</v>
@@ -4495,16 +4572,16 @@
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
-        <v>1.4496120429308179</v>
+        <v>1.6156231300658219</v>
       </c>
       <c r="B4" s="30">
-        <v>2.1701388888888888</v>
+        <v>1.7614397855638519</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -4516,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -4532,7 +4609,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -4544,7 +4621,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -4553,10 +4630,10 @@
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -4569,10 +4646,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -4581,10 +4658,10 @@
       <c r="A10" s="13"/>
       <c r="B10" s="15"/>
       <c r="C10" s="4">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -4592,12 +4669,8 @@
     <row r="11" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="5">
-        <v>49</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>35</v>
-      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
@@ -4635,16 +4708,16 @@
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -4653,10 +4726,1072 @@
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="4">
+        <v>7</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="4">
+        <v>25</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="4">
+        <v>47</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37">
+        <v>13</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>13</v>
+      </c>
+      <c r="B35" s="32">
+        <v>5</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="4">
+        <v>8</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="4">
+        <v>25</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="4">
+        <v>28</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="4">
         <v>49</v>
       </c>
+      <c r="D39" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>0.87347463070006415</v>
+      </c>
+      <c r="B4" s="30">
+        <v>0.87724137931034485</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="4">
+        <v>9</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
+        <v>49</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37">
+        <v>12</v>
+      </c>
+      <c r="B14" s="36">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
       <c r="D15" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="4">
+        <v>47</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37">
+        <v>13</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>13</v>
+      </c>
+      <c r="B35" s="32">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="4">
+        <v>8</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="4">
+        <v>25</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection sqref="A1:F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>1.291464287059001</v>
+      </c>
+      <c r="B4" s="30">
+        <v>2.305042833171421</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>35</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="4">
+        <v>9</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37">
+        <v>12</v>
+      </c>
+      <c r="B14" s="36">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <v>28</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="4">
+        <v>47</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -4750,10 +5885,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
-        <v>7</v>
-      </c>
-      <c r="B25" s="36"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="36">
+        <v>1</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="18"/>
       <c r="E25" s="9"/>
@@ -4848,16 +5983,16 @@
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B35" s="32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C35" s="4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -4865,48 +6000,32 @@
     <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="31"/>
-      <c r="C36" s="4">
-        <v>4</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>30</v>
-      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="31"/>
-      <c r="C37" s="4">
-        <v>7</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>44</v>
-      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="31"/>
-      <c r="C38" s="4">
-        <v>46</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="31"/>
-      <c r="C39" s="4">
-        <v>49</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
     </row>

</xml_diff>

<commit_message>
fixing the items for automation filling
</commit_message>
<xml_diff>
--- a/analysis/formats/QC_molds_daily_summary.xlsx
+++ b/analysis/formats/QC_molds_daily_summary.xlsx
@@ -3,25 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="944" firstSheet="0" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="daily" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="41" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="42" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="81" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="121" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="13" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="14" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="141" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
     <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+    <externalReference xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="AccessDatabase" hidden="1">"C:\Documents and Settings\Administrator\My Documents\BITUNIL\FINANCE\SAMEER\Cost StudyHB.mdb"</definedName>
@@ -48,7 +49,7 @@
     <definedName name="الاوزان">'[5]0'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'daily'!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" calcMode="manual" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2346,13 +2347,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2375,10 +2376,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -2436,21 +2437,50 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0</v>
+        <v>0.8839865446295861</v>
       </c>
       <c r="B4" s="30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+        <v>1.181604565290366</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>75QNED81 UR91</t>
+        </is>
+      </c>
+      <c r="AK4" t="n">
+        <v>462</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>527</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>527.5</v>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>75QNED81 UR91</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -2465,24 +2495,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>55C350K</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>بوتجاز  90 تصدير</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG75UP77set</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -2568,13 +2616,633 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
+        <v>9</v>
+      </c>
+      <c r="B14" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
+        </is>
+      </c>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="24" t="n"/>
+      <c r="B15" s="31" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="24" t="n"/>
+      <c r="B16" s="31" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="24" t="n"/>
+      <c r="B17" s="31" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="24" t="n"/>
+      <c r="B18" s="31" t="n"/>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="24" t="n"/>
+      <c r="B19" s="31" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="18" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="31" t="n"/>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="24" t="n"/>
+      <c r="B21" s="31" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="18" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A22" s="22" t="n"/>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="20" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+    </row>
+    <row r="23" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A23" s="35" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(الخفيفة)</t>
+        </is>
+      </c>
+      <c r="B23" s="27" t="n"/>
+      <c r="C23" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="29" t="n"/>
+      <c r="F23" s="29" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاقل من المواصفة </t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D24" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="37" t="n"/>
+      <c r="B25" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="18" t="n"/>
+      <c r="E25" s="9" t="n"/>
+      <c r="F25" s="9" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="24" t="n"/>
+      <c r="B26" s="31" t="n"/>
+      <c r="C26" s="4" t="n"/>
+      <c r="D26" s="18" t="n"/>
+      <c r="E26" s="9" t="n"/>
+      <c r="F26" s="9" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1">
+      <c r="A27" s="24" t="n"/>
+      <c r="B27" s="31" t="n"/>
+      <c r="C27" s="4" t="n"/>
+      <c r="D27" s="18" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="24" t="n"/>
+      <c r="B28" s="31" t="n"/>
+      <c r="C28" s="4" t="n"/>
+      <c r="D28" s="18" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="24" t="n"/>
+      <c r="B29" s="31" t="n"/>
+      <c r="C29" s="4" t="n"/>
+      <c r="D29" s="18" t="n"/>
+      <c r="E29" s="9" t="n"/>
+      <c r="F29" s="9" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="24" t="n"/>
+      <c r="B30" s="31" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="18" t="n"/>
+      <c r="E30" s="9" t="n"/>
+      <c r="F30" s="9" t="n"/>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="24" t="n"/>
+      <c r="B31" s="31" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="18" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A32" s="24" t="n"/>
+      <c r="B32" s="31" t="n"/>
+      <c r="C32" s="5" t="n"/>
+      <c r="D32" s="19" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A33" s="35" t="inlineStr">
+        <is>
+          <t>ثالثا : اوزان منتجات حقن الفوم(العالية)</t>
+        </is>
+      </c>
+      <c r="B33" s="27" t="n"/>
+      <c r="C33" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D33" s="29" t="n"/>
+      <c r="E33" s="29" t="n"/>
+    </row>
+    <row r="34" ht="18" customHeight="1" thickBot="1">
+      <c r="A34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات وفقا للمواصفة </t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">اوزان الاسطمبات الاعلي من المواصفة </t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D34" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1">
+      <c r="A35" s="23" t="n">
         <v>0</v>
       </c>
+      <c r="B35" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="n"/>
+      <c r="D35" s="18" t="n"/>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+    </row>
+    <row r="36" ht="18" customHeight="1">
+      <c r="A36" s="24" t="n"/>
+      <c r="B36" s="31" t="n"/>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="18" t="n"/>
+      <c r="E36" s="9" t="n"/>
+      <c r="F36" s="9" t="n"/>
+    </row>
+    <row r="37" ht="18" customHeight="1">
+      <c r="A37" s="24" t="n"/>
+      <c r="B37" s="31" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
+      <c r="E37" s="9" t="n"/>
+      <c r="F37" s="9" t="n"/>
+    </row>
+    <row r="38" ht="18" customHeight="1">
+      <c r="A38" s="24" t="n"/>
+      <c r="B38" s="31" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+    </row>
+    <row r="39" ht="18" customHeight="1">
+      <c r="A39" s="24" t="n"/>
+      <c r="B39" s="31" t="n"/>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="18" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+    </row>
+    <row r="40" ht="18" customHeight="1">
+      <c r="A40" s="24" t="n"/>
+      <c r="B40" s="31" t="n"/>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="18" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1">
+      <c r="A41" s="24" t="n"/>
+      <c r="B41" s="31" t="n"/>
+      <c r="C41" s="4" t="n"/>
+      <c r="D41" s="18" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A42" s="25" t="n"/>
+      <c r="B42" s="33" t="n"/>
+      <c r="C42" s="5" t="n"/>
+      <c r="D42" s="19" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM42"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.5703125" customWidth="1" min="3" max="3"/>
+    <col width="20.140625" customWidth="1" style="21" min="4" max="4"/>
+    <col width="28.85546875" customWidth="1" min="5" max="5"/>
+    <col width="31.85546875" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ملخص عن حالة تشغيل الماكينات  ليوم</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D1" s="16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="26" t="inlineStr">
+        <is>
+          <t>اولا : نسبة التالف على الماكينات</t>
+        </is>
+      </c>
+      <c r="B2" s="27" t="n"/>
+      <c r="C2" s="38" t="inlineStr">
+        <is>
+          <t>ملاحظات(نسبة التوالف لا تزيد عن 1.5 للماكينات الجديدة ، 2% للقديمة)</t>
+        </is>
+      </c>
+      <c r="D2" s="39" t="n"/>
+      <c r="E2" s="39" t="n"/>
+      <c r="F2" s="39" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على اجمالى الماكينات </t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">النسبة% على الماكينات الجديدة </t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.75" customHeight="1">
+      <c r="A4" s="34" t="n">
+        <v>0.9092596028947856</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>1.181598062953995</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>oled55cs6la</t>
+        </is>
+      </c>
+      <c r="AK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="5" ht="21.75" customHeight="1">
+      <c r="A5" s="24" t="n"/>
+      <c r="B5" s="31" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+    </row>
+    <row r="6" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>اعلي نسبة توالف</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG Nano80</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="21.75" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>LG32LM55-LM63</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+    </row>
+    <row r="8" ht="21.75" customHeight="1">
+      <c r="A8" s="13" t="n"/>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>قاعدة غسالة Lg</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+    </row>
+    <row r="9" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>لماكينة</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
+        <is>
+          <t>وسيط التوالف</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n"/>
+      <c r="D9" s="18" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="18" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A11" s="13" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="19" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A12" s="35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ثانيا : معدلات الاسطمبات </t>
+        </is>
+      </c>
+      <c r="B12" s="27" t="n"/>
+      <c r="C12" s="28" t="inlineStr">
+        <is>
+          <t>ملاحظات</t>
+        </is>
+      </c>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="29" t="n"/>
+      <c r="F12" s="29" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عدد الاسطمبات المحققة للمعدل </t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> عدد الاسطمبات الغيرمحققة للمعدل</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>رقم الماكينة</t>
+        </is>
+      </c>
+      <c r="D13" s="17" t="inlineStr">
+        <is>
+          <t>الصنف الغير مطابق</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>السبب</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>الاجراء التصحيحي لمعالجة السبب</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="37" t="n">
+        <v>14</v>
+      </c>
       <c r="B14" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="18" t="n"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>جانب حماية يمين / شمال</t>
+        </is>
+      </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
@@ -2691,9 +3359,11 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="37" t="n"/>
+      <c r="A25" s="37" t="n">
+        <v>14</v>
+      </c>
       <c r="B25" s="36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
@@ -2703,8 +3373,14 @@
     <row r="26" ht="18" customHeight="1">
       <c r="A26" s="24" t="n"/>
       <c r="B26" s="31" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="18" t="n"/>
+      <c r="C26" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>جانب حماية يمين / شمال</t>
+        </is>
+      </c>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
     </row>
@@ -2804,12 +3480,8 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" s="32" t="n">
-        <v>0</v>
-      </c>
+      <c r="A35" s="23" t="n"/>
+      <c r="B35" s="32" t="n"/>
       <c r="C35" s="4" t="n"/>
       <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
@@ -2901,10 +3573,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="A14:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2924,10 +3596,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -2984,18 +3656,41 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="34" t="n"/>
-      <c r="B4" s="30" t="n"/>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+      <c r="A4" s="34" t="n">
+        <v>0.5997269899523351</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>0.4977842530200935</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>144</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>165</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>245</v>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>240</v>
+      </c>
+      <c r="D5" s="18" t="n">
+        <v>274</v>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -3010,24 +3705,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>صندوق 10 ك فلات</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم سخان غاز 10 لتر</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -3113,29 +3826,47 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>0</v>
+        <v>110.75</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="18" t="n"/>
+        <v>97</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 10بنى سويف</t>
+        </is>
+      </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
@@ -3238,7 +3969,7 @@
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="37" t="n"/>
       <c r="B25" s="36" t="n">
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="18" t="n"/>
@@ -3349,12 +4080,8 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" s="32" t="n">
-        <v>0</v>
-      </c>
+      <c r="A35" s="23" t="n"/>
+      <c r="B35" s="32" t="n"/>
       <c r="C35" s="4" t="n"/>
       <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
@@ -3446,10 +4173,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3469,10 +4196,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -3529,12 +4256,30 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="34" t="n"/>
-      <c r="B4" s="30" t="n"/>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+      <c r="A4" s="34" t="n">
+        <v>0.7181006238499169</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>0.6373486297004461</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>LG LG 55QNED81-UR91</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
@@ -3658,29 +4403,47 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="18" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
@@ -3781,12 +4544,20 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="37" t="n"/>
+      <c r="A25" s="37" t="n">
+        <v>9</v>
+      </c>
       <c r="B25" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="18" t="n"/>
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>OLED65A2</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -3894,12 +4665,8 @@
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="B35" s="32" t="n">
-        <v>0</v>
-      </c>
+      <c r="A35" s="23" t="n"/>
+      <c r="B35" s="32" t="n"/>
       <c r="C35" s="4" t="n"/>
       <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
@@ -3991,10 +4758,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4014,10 +4781,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -4074,18 +4841,42 @@
       </c>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="34" t="n"/>
-      <c r="B4" s="30" t="n"/>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+      <c r="A4" s="34" t="n">
+        <v>0.5742630587063969</v>
+      </c>
+      <c r="B4" s="30" t="n">
+        <v>0.5458618622408734</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>طقم تغليف فلتر</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -4100,24 +4891,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>LG LG 55QNED81-UR91</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -4203,29 +5012,47 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="18" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
@@ -4326,12 +5153,20 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="37" t="n"/>
+      <c r="A25" s="37" t="n">
+        <v>12</v>
+      </c>
       <c r="B25" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="18" t="n"/>
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>OLED65A2</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -4440,7 +5275,7 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B35" s="32" t="n">
         <v>0</v>
@@ -4504,7 +5339,10 @@
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
+      <c r="F42" s="10">
+        <f>+F1:AA42</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4536,10 +5374,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4559,10 +5397,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -4620,13 +5458,13 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>1.015486164001016</v>
+        <v>0.9413120737681299</v>
       </c>
       <c r="B4" s="30" t="n">
-        <v>0.8390089823314579</v>
+        <v>1.273172437915355</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
@@ -4635,12 +5473,26 @@
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>LG LG 55QNED81-UR91</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -4655,16 +5507,28 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
@@ -4758,17 +5622,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -4778,11 +5642,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>علبة صندوق سمك 20 ك فلات الجديدة</t>
+          <t>شارب 14</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -4792,11 +5656,11 @@
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D16" s="18" t="inlineStr">
         <is>
-          <t>زوايا غسالة كليوباترا</t>
+          <t>فوم طقم رويال جاز المعدل</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -4805,56 +5669,32 @@
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="31" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D17" s="18" t="inlineStr">
-        <is>
-          <t>صندوق سمك 25 ك</t>
-        </is>
-      </c>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="31" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="D18" s="18" t="inlineStr">
-        <is>
-          <t>شارب 14</t>
-        </is>
-      </c>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
       <c r="A19" s="24" t="n"/>
       <c r="B19" s="31" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D19" s="18" t="inlineStr">
-        <is>
-          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
       <c r="A20" s="24" t="n"/>
       <c r="B20" s="31" t="n"/>
-      <c r="C20" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D20" s="18" t="inlineStr">
-        <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-        </is>
-      </c>
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="18" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
     </row>
@@ -4924,17 +5764,13 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="37" t="n">
-        <v>13</v>
-      </c>
-      <c r="B25" s="36" t="n"/>
-      <c r="C25" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D25" s="18" t="inlineStr">
-        <is>
-          <t>LG 65NANO075 SIDE</t>
-        </is>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B25" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="18" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -5041,19 +5877,19 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1">
+    <row r="35" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="23" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="32" t="n">
         <v>4</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>فوم حمايةالعداد2</t>
+          <t xml:space="preserve">صندوق سمك 25 ك  </t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -5063,11 +5899,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>شارب 14</t>
+          <t>LG LG 55QNED81-UR91</t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -5077,11 +5913,11 @@
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="31" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
@@ -5090,8 +5926,14 @@
     <row r="38" ht="18" customHeight="1">
       <c r="A38" s="24" t="n"/>
       <c r="B38" s="31" t="n"/>
-      <c r="C38" s="4" t="n"/>
-      <c r="D38" s="18" t="n"/>
+      <c r="C38" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D38" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
@@ -5157,7 +5999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AJ42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5180,10 +6022,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -5241,31 +6083,39 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.5863192182410424</v>
+        <v>0.9413120737681299</v>
       </c>
       <c r="B4" s="30" t="n">
-        <v>0.6479902557856273</v>
+        <v>1.273172437915355</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>FRONT 43LM55</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>LG LG 55QNED81-UR91</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -5282,16 +6132,28 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>شارب 14</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
@@ -5385,17 +6247,17 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
-          <t>فوم طقم رويال جاز المعدل</t>
+          <t>صندوق سمك 25 ك</t>
         </is>
       </c>
       <c r="E14" s="9" t="n"/>
@@ -5405,11 +6267,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>زوايا غسالة كليوباترا</t>
+          <t>شارب 14</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -5419,11 +6281,11 @@
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D16" s="18" t="inlineStr">
         <is>
-          <t>صندوق سمك 25 ك</t>
+          <t>فوم طقم رويال جاز المعدل</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -5432,42 +6294,24 @@
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="31" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="D17" s="18" t="inlineStr">
-        <is>
-          <t>شارب 14</t>
-        </is>
-      </c>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="31" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D18" s="18" t="inlineStr">
-        <is>
-          <t>كفر سخان فرنساوى 085/قاعده سخان فرنساوى 086</t>
-        </is>
-      </c>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
       <c r="A19" s="24" t="n"/>
       <c r="B19" s="31" t="n"/>
-      <c r="C19" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D19" s="18" t="inlineStr">
-        <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-        </is>
-      </c>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="18" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
     </row>
@@ -5545,7 +6389,7 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="37" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="36" t="n"/>
       <c r="C25" s="4" t="n"/>
@@ -5658,61 +6502,37 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="C35" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="D35" s="18" t="inlineStr">
-        <is>
-          <t>فوم حمايةالعداد2</t>
-        </is>
-      </c>
+      <c r="C35" s="4" t="n"/>
+      <c r="D35" s="18" t="n"/>
       <c r="E35" s="9" t="n"/>
       <c r="F35" s="9" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="31" t="n"/>
-      <c r="C36" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="D36" s="18" t="inlineStr">
-        <is>
-          <t>فوم كوش 152</t>
-        </is>
-      </c>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="18" t="n"/>
       <c r="E36" s="9" t="n"/>
       <c r="F36" s="9" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="31" t="n"/>
-      <c r="C37" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="D37" s="18" t="inlineStr">
-        <is>
-          <t>شارب 14</t>
-        </is>
-      </c>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="18" t="n"/>
       <c r="E37" s="9" t="n"/>
       <c r="F37" s="9" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
       <c r="A38" s="24" t="n"/>
       <c r="B38" s="31" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D38" s="18" t="inlineStr">
-        <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-        </is>
-      </c>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
@@ -5778,10 +6598,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AQ42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F42"/>
+    <sheetView rightToLeft="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -5801,10 +6621,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -5862,31 +6682,54 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v>0.5528275503235667</v>
+        <v>1.070072488781498</v>
       </c>
       <c r="B4" s="30" t="n">
-        <v>0.7258064516129032</v>
+        <v>1.027625784065128</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="18" t="inlineStr">
         <is>
-          <t>قاعدة غسالة Lg</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
+      <c r="AK4" t="n">
+        <v>897</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1021</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1021.166666666667</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
       <c r="C5" s="4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" s="18" t="inlineStr">
         <is>
-          <t>LG65UP77_TB</t>
+          <t>LG LG 55QNED81-UR91</t>
         </is>
       </c>
       <c r="E5" s="9" t="n"/>
@@ -5903,16 +6746,28 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>فوم حمايةالعداد2</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 23ك فلات</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
@@ -6006,13 +6861,13 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D14" s="18" t="inlineStr">
         <is>
@@ -6026,11 +6881,11 @@
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
       <c r="C15" s="4" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>Stop Coller S4</t>
+          <t>بوتجاز  90 تصدير</t>
         </is>
       </c>
       <c r="E15" s="9" t="n"/>
@@ -6040,11 +6895,11 @@
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
       <c r="C16" s="4" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D16" s="18" t="inlineStr">
         <is>
-          <t>شارب 14</t>
+          <t>فوم طقم رويال جاز المعدل</t>
         </is>
       </c>
       <c r="E16" s="9" t="n"/>
@@ -6053,28 +6908,16 @@
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="24" t="n"/>
       <c r="B17" s="31" t="n"/>
-      <c r="C17" s="4" t="n">
-        <v>47</v>
-      </c>
-      <c r="D17" s="18" t="inlineStr">
-        <is>
-          <t>كفر سخان فرنساوى 085/قاعده سخان فر</t>
-        </is>
-      </c>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="18" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
       <c r="A18" s="24" t="n"/>
       <c r="B18" s="31" t="n"/>
-      <c r="C18" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D18" s="18" t="inlineStr">
-        <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-        </is>
-      </c>
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="18" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
     </row>
@@ -6160,11 +7003,19 @@
     </row>
     <row r="25" ht="18" customHeight="1">
       <c r="A25" s="37" t="n">
-        <v>10</v>
-      </c>
-      <c r="B25" s="36" t="n"/>
-      <c r="C25" s="4" t="n"/>
-      <c r="D25" s="18" t="n"/>
+        <v>14</v>
+      </c>
+      <c r="B25" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 23ك فلات</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -6271,19 +7122,19 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18" customHeight="1">
+    <row r="35" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="23" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B35" s="32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>قاعدة وزوايا كولدير ميلو</t>
+          <t>LG65UP77_TB</t>
         </is>
       </c>
       <c r="E35" s="9" t="n"/>
@@ -6293,11 +7144,11 @@
       <c r="A36" s="24" t="n"/>
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="4" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D36" s="18" t="inlineStr">
         <is>
-          <t>فوم كوش 152</t>
+          <t xml:space="preserve">LG LG 55QNED81-UR91 </t>
         </is>
       </c>
       <c r="E36" s="9" t="n"/>
@@ -6307,11 +7158,11 @@
       <c r="A37" s="24" t="n"/>
       <c r="B37" s="31" t="n"/>
       <c r="C37" s="4" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>Stop Coller S4</t>
+          <t>فوم حمايةالعداد2</t>
         </is>
       </c>
       <c r="E37" s="9" t="n"/>
@@ -6320,42 +7171,24 @@
     <row r="38" ht="18" customHeight="1">
       <c r="A38" s="24" t="n"/>
       <c r="B38" s="31" t="n"/>
-      <c r="C38" s="4" t="n">
-        <v>30</v>
-      </c>
-      <c r="D38" s="18" t="inlineStr">
-        <is>
-          <t>شارب 14</t>
-        </is>
-      </c>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="18" t="n"/>
       <c r="E38" s="9" t="n"/>
       <c r="F38" s="9" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
       <c r="A39" s="24" t="n"/>
       <c r="B39" s="31" t="n"/>
-      <c r="C39" s="4" t="n">
-        <v>48</v>
-      </c>
-      <c r="D39" s="18" t="inlineStr">
-        <is>
-          <t>طقم سخان نبتون ذو 4 اطقم</t>
-        </is>
-      </c>
+      <c r="C39" s="4" t="n"/>
+      <c r="D39" s="18" t="n"/>
       <c r="E39" s="9" t="n"/>
       <c r="F39" s="9" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
       <c r="A40" s="24" t="n"/>
       <c r="B40" s="31" t="n"/>
-      <c r="C40" s="4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D40" s="18" t="inlineStr">
-        <is>
-          <t>قاعدة ولوحة تحكم غسالة كيلوباترا</t>
-        </is>
-      </c>
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="18" t="n"/>
       <c r="E40" s="9" t="n"/>
       <c r="F40" s="9" t="n"/>
     </row>
@@ -6405,10 +7238,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -6428,10 +7261,10 @@
         </is>
       </c>
       <c r="B1" s="2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="16" t="n">
         <v>2023</v>
@@ -6489,21 +7322,50 @@
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="34" t="n">
-        <v/>
+        <v>0.8839865446295861</v>
       </c>
       <c r="B4" s="30" t="n">
-        <v/>
-      </c>
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="18" t="n"/>
+        <v>1.181604565290366</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>LG65UP77_TB</t>
+        </is>
+      </c>
       <c r="E4" s="9" t="n"/>
       <c r="F4" s="9" t="n"/>
+      <c r="AI4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>75QNED81 UR91</t>
+        </is>
+      </c>
+      <c r="AK4" t="n">
+        <v>462</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>527</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>527.5</v>
+      </c>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="24" t="n"/>
       <c r="B5" s="31" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="18" t="n"/>
+      <c r="C5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="inlineStr">
+        <is>
+          <t>75QNED81 UR91</t>
+        </is>
+      </c>
       <c r="E5" s="9" t="n"/>
       <c r="F5" s="9" t="n"/>
     </row>
@@ -6518,24 +7380,42 @@
           <t>اعلي نسبة توالف</t>
         </is>
       </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="18" t="n"/>
+      <c r="C6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18" t="inlineStr">
+        <is>
+          <t>55C350K</t>
+        </is>
+      </c>
       <c r="E6" s="9" t="n"/>
       <c r="F6" s="9" t="n"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="13" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="4" t="n"/>
-      <c r="D7" s="18" t="n"/>
+      <c r="C7" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" s="18" t="inlineStr">
+        <is>
+          <t>بوتجاز  90 تصدير</t>
+        </is>
+      </c>
       <c r="E7" s="9" t="n"/>
       <c r="F7" s="9" t="n"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="13" t="n"/>
       <c r="B8" s="14" t="n"/>
-      <c r="C8" s="4" t="n"/>
-      <c r="D8" s="18" t="n"/>
+      <c r="C8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18" t="inlineStr">
+        <is>
+          <t>LG75UP77set</t>
+        </is>
+      </c>
       <c r="E8" s="9" t="n"/>
       <c r="F8" s="9" t="n"/>
     </row>
@@ -6621,29 +7501,47 @@
     </row>
     <row r="14" ht="18" customHeight="1">
       <c r="A14" s="37" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B14" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="n"/>
-      <c r="D14" s="18" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>صندوق سمك 25 ك</t>
+        </is>
+      </c>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1">
       <c r="A15" s="24" t="n"/>
       <c r="B15" s="31" t="n"/>
-      <c r="C15" s="4" t="n"/>
-      <c r="D15" s="18" t="n"/>
+      <c r="C15" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>زوايا غسالة كليوباترا</t>
+        </is>
+      </c>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
     </row>
     <row r="16" ht="18" customHeight="1">
       <c r="A16" s="24" t="n"/>
       <c r="B16" s="31" t="n"/>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="18" t="n"/>
+      <c r="C16" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>فوم طقم رويال جاز المعدل</t>
+        </is>
+      </c>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
     </row>
@@ -6744,12 +7642,18 @@
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="37" t="n"/>
+      <c r="A25" s="37" t="n">
+        <v>11</v>
+      </c>
       <c r="B25" s="36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="4" t="n"/>
-      <c r="D25" s="18" t="n"/>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>75QNED81 UR91</t>
+        </is>
+      </c>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
     </row>
@@ -6858,7 +7762,7 @@
     </row>
     <row r="35" ht="18" customHeight="1">
       <c r="A35" s="23" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B35" s="32" t="n">
         <v>0</v>
@@ -6922,7 +7826,10 @@
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="19" t="n"/>
       <c r="E42" s="10" t="n"/>
-      <c r="F42" s="10" t="n"/>
+      <c r="F42" s="10">
+        <f>+A1A1:F42</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>